<commit_message>
20250322_best so far. no bias towards red/blue_first bet on this
</commit_message>
<xml_diff>
--- a/data/ufc_upcoming_events.xlsx
+++ b/data/ufc_upcoming_events.xlsx
@@ -648,72 +648,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/67f7163e536d62e2</t>
+          <t>http://ufcstats.com/fight-details/371ed8497799998e</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Marvin Vettori</t>
+          <t>Leon Edwards</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Roman Dolidze</t>
+          <t>Sean Brady</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Middleweight Bout</t>
+          <t>Welterweight Bout</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>17:22</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>56%</t>
+          <t>53%</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Sep 20, 1993</t>
+          <t>Aug 25, 1991</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>6' 0"</t>
+          <t>6' 2"</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/7acbb0972e75281a</t>
+          <t>http://ufcstats.com/fighter-details/f1fac969a1d70b08</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>"The Italian Dream"</t>
+          <t>"Rocky"</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -728,78 +728,78 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>4.24</t>
+          <t>2.37</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>4.56</t>
+          <t>2.68</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>53%</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>0.4</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>36%</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>69%</t>
+          <t>65%</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>1.66</t>
+          <t>1.25</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>185 lbs.</t>
+          <t>170 lbs.</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>19-7-1</t>
+          <t>22-4-0 (1 NC)</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>13:58</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>Jul 15, 1988</t>
+          <t>Nov 23, 1992</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>6' 2"</t>
+          <t>5' 10"</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/327d5f279895110d</t>
+          <t>http://ufcstats.com/fighter-details/45f7cb591c3ab00b</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>76"</t>
+          <t>72"</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
@@ -809,331 +809,327 @@
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>3.38</t>
+          <t>3.18</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>3.16</t>
+          <t>4.09</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>42%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>1.1</t>
+          <t>0.9</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>42%</t>
+          <t>52%</t>
         </is>
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="AN2" t="inlineStr">
         <is>
-          <t>1.33</t>
+          <t>3.49</t>
         </is>
       </c>
       <c r="AO2" t="inlineStr">
         <is>
-          <t>185 lbs.</t>
+          <t>170 lbs.</t>
         </is>
       </c>
       <c r="AP2" t="inlineStr">
         <is>
-          <t>14-3-0</t>
+          <t>17-1-0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/c83133ee114945ed</t>
+          <t>http://ufcstats.com/fight-details/6d9ea9f436ed354d</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Chidi Njokuani</t>
+          <t>Jan Blachowicz</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Elizeu Zaleski dos Santos</t>
+          <t>Carlos Ulberg</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Welterweight Bout</t>
+          <t>Light Heavyweight Bout</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>9:42</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
+          <t>53%</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Feb 24, 1983</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>6' 2"</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>http://ufcstats.com/fighter-details/99df7d0a2a08a8a8</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>78"</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Orthodox</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2.91</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>3.41</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>68%</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>1.09</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>205 lbs.</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>29-10-1</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>6:57</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Nov 07, 1990</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>6' 4"</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>http://ufcstats.com/fighter-details/9014c02eff8b3d62</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>"Black Jag"</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>77"</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>Orthodox</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>4.27</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>7.20</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
           <t>56%</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Dec 31, 1988</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>6' 3"</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>http://ufcstats.com/fighter-details/c68c68efaa5ca6ef</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>"Bang Bang"</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>80"</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Orthodox</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>2.67</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>4.59</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>63%</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
+      <c r="AK3" t="inlineStr">
         <is>
           <t>0.2</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>170 lbs.</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>24-10-0 (1 NC)</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>11:59</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>56%</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>Dec 11, 1986</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>5' 11"</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>http://ufcstats.com/fighter-details/8adcbd525fab8d9b</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>"Capoeira"</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>73"</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>Orthodox</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>3.41</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>4.33</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>41%</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>20%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>68%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="AN3" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>0.72</t>
         </is>
       </c>
       <c r="AO3" t="inlineStr">
         <is>
-          <t>170 lbs.</t>
+          <t>205 lbs.</t>
         </is>
       </c>
       <c r="AP3" t="inlineStr">
         <is>
-          <t>25-8-1</t>
+          <t>12-1-0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/d8f40b82364b6411</t>
+          <t>http://ufcstats.com/fight-details/96c6be6b22385967</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Alexander Hernandez</t>
+          <t>Gunnar Nelson</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Kurt Holobaugh</t>
+          <t>Kevin Holland</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Lightweight Bout</t>
+          <t>Welterweight Bout</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>10:02</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>57%</t>
+          <t>49%</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Oct 01, 1992</t>
+          <t>Jul 28, 1988</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>5' 9"</t>
+          <t>5' 11"</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/262a7d06203657e6</t>
+          <t>http://ufcstats.com/fighter-details/fd55393021a8c255</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>"The Great Ape"</t>
+          <t>"Gunni"</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -1143,299 +1139,299 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>1.84</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>61%</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>59%</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>66%</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>1.90</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>170 lbs.</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>19-5-1</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>10:18</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Nov 05, 1992</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>6' 3"</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>http://ufcstats.com/fighter-details/3a46b268013afede</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>"Trailblazer"</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>81"</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
           <t>Orthodox</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>4.61</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>4.43</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>41%</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>0.1</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>29%</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>71%</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>0.95</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>155 lbs.</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>15-8-0</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>11:02</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>47%</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>Sep 08, 1986</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>5' 11"</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>http://ufcstats.com/fighter-details/a7151778b3381036</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>"The Hurt"</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>70"</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>Orthodox</t>
-        </is>
-      </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>4.35</t>
+          <t>3.22</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>4.63</t>
+          <t>4.22</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>49%</t>
         </is>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>38%</t>
         </is>
       </c>
       <c r="AM4" t="inlineStr">
         <is>
-          <t>42%</t>
+          <t>53%</t>
         </is>
       </c>
       <c r="AN4" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.82</t>
         </is>
       </c>
       <c r="AO4" t="inlineStr">
         <is>
-          <t>155 lbs.</t>
+          <t>170 lbs.</t>
         </is>
       </c>
       <c r="AP4" t="inlineStr">
         <is>
-          <t>22-8-0 (1 NC)</t>
+          <t>26-13-0 (1 NC)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/ab1aa23060d4e87b</t>
+          <t>http://ufcstats.com/fight-details/b5b4b69bccb9ff4a</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Da'Mon Blackshear</t>
+          <t>Molly McCann</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Cody Gibson</t>
+          <t>Alexia Thainara</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Bantamweight Bout</t>
+          <t>Women's Strawweight Bout</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>8:54</t>
+          <t>10:38</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
+          <t>62%</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>May 04, 1990</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>5' 4"</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>http://ufcstats.com/fighter-details/51018a31ddf31eb2</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>"Meatball"</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>62"</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Orthodox</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>4.72</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>5.39</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
           <t>49%</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Aug 12, 1994</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>5' 10"</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>http://ufcstats.com/fighter-details/da22387a0407a2dc</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>"The Monster"</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>72"</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Switch</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>4.06</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>4.30</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>47%</t>
-        </is>
-      </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>37%</t>
+          <t>36%</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>68%</t>
+          <t>39%</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>2.17</t>
+          <t>1.84</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>135 lbs.</t>
+          <t>115 lbs.</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>15-7-1</t>
+          <t>14-7-0</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>11:12</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>57%</t>
+          <t>71%</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>Sep 11, 1987</t>
+          <t>Nov 20, 1995</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>5' 10"</t>
+          <t>5' 4"</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/700a674c042b7a96</t>
+          <t>http://ufcstats.com/fighter-details/545092d13c67aa49</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>"The Renegade"</t>
+          <t>"Burguesinha"</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>71"</t>
+          <t>67"</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
@@ -1445,140 +1441,144 @@
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>3.36</t>
+          <t>3.07</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>3.47</t>
+          <t>6.73</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>44%</t>
+          <t>39%</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>0.7</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>68%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="AN5" t="inlineStr">
         <is>
-          <t>2.18</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="AO5" t="inlineStr">
         <is>
-          <t>135 lbs.</t>
+          <t>115 lbs.</t>
         </is>
       </c>
       <c r="AP5" t="inlineStr">
         <is>
-          <t>22-10-0</t>
+          <t>11-1-0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/e56403718205b494</t>
+          <t>http://ufcstats.com/fight-details/8e6640c007ad603d</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Diyar Nurgozhay</t>
+          <t>Jordan Vucenic</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Brendson Ribeiro</t>
+          <t>Chris Duncan</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Light Heavyweight Bout</t>
+          <t>Lightweight Bout</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>8:32</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Apr 22, 1997</t>
+          <t>Mar 02, 1996</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>6' 2"</t>
+          <t>5' 10"</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/709fadb644ee3f51</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr"/>
+          <t>http://ufcstats.com/fighter-details/6d38e41efa47a72d</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>"The Epidemic"</t>
+        </is>
+      </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>74"</t>
+          <t>73"</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Southpaw</t>
+          <t>Orthodox</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2.70</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>3.52</t>
+          <t>2.27</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>52%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -1603,47 +1603,47 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>205 lbs.</t>
+          <t>155 lbs.</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>10-0-0</t>
+          <t>13-3-0</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>8:52</t>
+          <t>7:05</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>48%</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>Sep 08, 1996</t>
+          <t>May 10, 1993</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>6' 3"</t>
+          <t>5' 10"</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/49edd0d90f60fb7d</t>
+          <t>http://ufcstats.com/fighter-details/fd406a32a6fb3a29</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>"The Gorilla"</t>
+          <t>"The Problem"</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>81"</t>
+          <t>71"</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
@@ -1653,84 +1653,84 @@
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>3.92</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>3.16</t>
+          <t>4.70</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>42%</t>
+          <t>46%</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>0.4</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>37%</t>
         </is>
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>33%</t>
         </is>
       </c>
       <c r="AN6" t="inlineStr">
         <is>
-          <t>1.27</t>
+          <t>3.53</t>
         </is>
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>205 lbs.</t>
+          <t>155 lbs.</t>
         </is>
       </c>
       <c r="AP6" t="inlineStr">
         <is>
-          <t>16-7-0 (1 NC)</t>
+          <t>12-2-0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/36db86c39ed09997</t>
+          <t>http://ufcstats.com/fight-details/9779eb1aae1d4654</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>SeungWoo Choi</t>
+          <t>Nathaniel Wood</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Kevin Vallejos</t>
+          <t>Morgan Charriere</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1740,37 +1740,37 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>13:08</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>47%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Nov 03, 1992</t>
+          <t>May 08, 1993</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>6' 0"</t>
+          <t>5' 6"</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/a68575214ecad140</t>
+          <t>http://ufcstats.com/fighter-details/329e403448756217</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>"Sting"</t>
+          <t>"The Prospect"</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>74"</t>
+          <t>69"</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1780,37 +1780,37 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>3.12</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>3.51</t>
+          <t>5.75</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>39%</t>
+          <t>51%</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>48%</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>0.86</t>
+          <t>1.56</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
@@ -1820,57 +1820,57 @@
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>11-7-0</t>
+          <t>20-6-0</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>8:42</t>
+          <t>8:06</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>Dec 08, 2001</t>
+          <t>Oct 26, 1995</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>5' 7"</t>
+          <t>5' 8"</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/239d8e5359022f3b</t>
+          <t>http://ufcstats.com/fighter-details/5b03b61f9d90125e</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>"El Chino"</t>
+          <t>"The Last Pirate"</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>68"</t>
+          <t>69"</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>Switch</t>
+          <t>Orthodox</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>5.81</t>
+          <t>3.74</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
-          <t>6.85</t>
+          <t>3.87</t>
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
@@ -1880,22 +1880,22 @@
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="AN7" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>2.47</t>
         </is>
       </c>
       <c r="AO7" t="inlineStr">
@@ -1905,54 +1905,54 @@
       </c>
       <c r="AP7" t="inlineStr">
         <is>
-          <t>14-1-0</t>
+          <t>20-10-1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/74bc22b367cca118</t>
+          <t>http://ufcstats.com/fight-details/2a1071689c3af9df</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Waldo Cortes-Acosta</t>
+          <t>Jai Herbert</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Ryan Spann</t>
+          <t>Chris Padilla</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Heavyweight Bout</t>
+          <t>Lightweight Bout</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>11:40</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1962,27 +1962,27 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Oct 03, 1991</t>
+          <t>May 13, 1988</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>6' 4"</t>
+          <t>6' 1"</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/fc08099550072fe4</t>
+          <t>http://ufcstats.com/fighter-details/4c88a1db5a46c6a4</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>"Salsa Boy"</t>
+          <t>"Black Country Banger"</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>78"</t>
+          <t>77"</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1992,82 +1992,82 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>3.60</t>
+          <t>3.37</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>5.64</t>
+          <t>3.16</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>48%</t>
+          <t>42%</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>0.55</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>260 lbs.</t>
+          <t>155 lbs.</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>12-1-0</t>
+          <t>13-5-1</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>5:19</t>
+          <t>6:54</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>43%</t>
+          <t>46%</t>
         </is>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>Aug 24, 1991</t>
+          <t>Sep 14, 1995</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>6' 5"</t>
+          <t>5' 9"</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/a67f5afa8d6a1b80</t>
+          <t>http://ufcstats.com/fighter-details/06626b6287e1ae1e</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>"Superman"</t>
+          <t>"Taco"</t>
         </is>
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>79"</t>
+          <t>74"</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr">
@@ -2077,236 +2077,232 @@
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>3.90</t>
+          <t>4.93</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr">
         <is>
-          <t>3.30</t>
+          <t>5.80</t>
         </is>
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>61%</t>
         </is>
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>1.7</t>
+          <t>1.1</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>35%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="AM8" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="AN8" t="inlineStr">
         <is>
-          <t>1.32</t>
+          <t>3.26</t>
         </is>
       </c>
       <c r="AO8" t="inlineStr">
         <is>
-          <t>205 lbs.</t>
+          <t>155 lbs.</t>
         </is>
       </c>
       <c r="AP8" t="inlineStr">
         <is>
-          <t>22-10-0</t>
+          <t>15-6-0</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/29d9c5a3f2b78903</t>
+          <t>http://ufcstats.com/fight-details/e5a88f5c686173c4</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>SuYoung You</t>
+          <t>Lone'er Kavanagh</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>AJ Cunningham</t>
+          <t>Felipe dos Santos</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Bantamweight Bout</t>
+          <t>Flyweight Bout</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
+          <t>8:43</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>67%</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Jun 09, 1999</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>5' 4"</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>http://ufcstats.com/fighter-details/bb2c3c3a466224af</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>67"</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Orthodox</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>3.45</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>3.62</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>43%</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>125 lbs.</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>8-0-0</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
           <t>15:00</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>72%</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Dec 11, 1995</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>5' 6"</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>http://ufcstats.com/fighter-details/a474aade8eb3a8f0</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>"Yoo-Jitsu"</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>65"</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>41%</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>Sep 11, 2000</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>5' 7"</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>http://ufcstats.com/fighter-details/5cdf5339728f580d</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>"Lipe Detona"</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>70"</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
         <is>
           <t>Orthodox</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>1.40</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>2.11</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>42%</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>3.78</t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>3.87</t>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>37%</t>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
         <is>
           <t>0.3</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>58%</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>66%</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>4.67</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>135 lbs.</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>14-3-0 (2 NC)</t>
-        </is>
-      </c>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t>6:51</t>
-        </is>
-      </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>48%</t>
-        </is>
-      </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>Sep 07, 1994</t>
-        </is>
-      </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>5' 10"</t>
-        </is>
-      </c>
-      <c r="AD9" t="inlineStr">
-        <is>
-          <t>http://ufcstats.com/fighter-details/d1053e55f00e53fe</t>
-        </is>
-      </c>
-      <c r="AE9" t="inlineStr">
-        <is>
-          <t>"The Savage"</t>
-        </is>
-      </c>
-      <c r="AF9" t="inlineStr">
-        <is>
-          <t>71"</t>
-        </is>
-      </c>
-      <c r="AG9" t="inlineStr">
-        <is>
-          <t>Orthodox</t>
-        </is>
-      </c>
-      <c r="AH9" t="inlineStr">
-        <is>
-          <t>11.90</t>
-        </is>
-      </c>
-      <c r="AI9" t="inlineStr">
-        <is>
-          <t>7.66</t>
-        </is>
-      </c>
-      <c r="AJ9" t="inlineStr">
-        <is>
-          <t>29%</t>
-        </is>
-      </c>
-      <c r="AK9" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="AL9" t="inlineStr">
         <is>
           <t>0%</t>
@@ -2314,7 +2310,7 @@
       </c>
       <c r="AM9" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>14%</t>
         </is>
       </c>
       <c r="AN9" t="inlineStr">
@@ -2324,89 +2320,89 @@
       </c>
       <c r="AO9" t="inlineStr">
         <is>
-          <t>135 lbs.</t>
+          <t>125 lbs.</t>
         </is>
       </c>
       <c r="AP9" t="inlineStr">
         <is>
-          <t>11-4-0</t>
+          <t>8-2-0 (1 NC)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/cb3eb07b7152366e</t>
+          <t>http://ufcstats.com/fight-details/dd229687cb62c871</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Carlos Vera</t>
+          <t>Marcin Tybura</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Josias Musasa</t>
+          <t>Mick Parkin</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Bantamweight Bout</t>
+          <t>Heavyweight Bout</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>11:04</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>55%</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Nov 05, 1987</t>
+          <t>Nov 09, 1985</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>5' 6"</t>
+          <t>6' 3"</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/07f959e6596307bb</t>
+          <t>http://ufcstats.com/fighter-details/c9cf753cfdf77fc2</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>"Pequeno"</t>
+          <t>"Tybur"</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>69"</t>
+          <t>78"</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -2416,837 +2412,833 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2.53</t>
+          <t>3.26</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>0.80</t>
+          <t>3.57</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>48%</t>
+          <t>49%</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>33%</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1.42</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>135 lbs.</t>
+          <t>249 lbs.</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>11-4-0</t>
+          <t>26-9-0</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>10:04</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>27%</t>
+          <t>58%</t>
         </is>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>Oct 10, 1998</t>
+          <t>Oct 02, 1995</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>5' 8"</t>
+          <t>6' 4"</t>
         </is>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/723b64c0e9a8f348</t>
-        </is>
-      </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>"The KO Wizard"</t>
-        </is>
-      </c>
+          <t>http://ufcstats.com/fighter-details/0d5cc0170c1a7e71</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>74"</t>
+          <t>79"</t>
         </is>
       </c>
       <c r="AG10" t="inlineStr">
         <is>
-          <t>Southpaw</t>
+          <t>Orthodox</t>
         </is>
       </c>
       <c r="AH10" t="inlineStr">
         <is>
-          <t>4.53</t>
+          <t>4.15</t>
         </is>
       </c>
       <c r="AI10" t="inlineStr">
         <is>
-          <t>3.33</t>
+          <t>4.91</t>
         </is>
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
-          <t>44%</t>
+          <t>52%</t>
         </is>
       </c>
       <c r="AK10" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>41%</t>
         </is>
       </c>
       <c r="AM10" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="AN10" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>1.49</t>
         </is>
       </c>
       <c r="AO10" t="inlineStr">
         <is>
-          <t>135 lbs.</t>
+          <t>265 lbs.</t>
         </is>
       </c>
       <c r="AP10" t="inlineStr">
         <is>
-          <t>8-0-0</t>
+          <t>10-0-0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/5fa6543868367f4b</t>
+          <t>http://ufcstats.com/fight-details/8af2b589d5e9c1ae</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Stephanie Luciano</t>
+          <t>Christian Leroy Duncan</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Sam Hughes</t>
+          <t>Andrey Pulyaev</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Women's Strawweight Bout</t>
+          <t>Middleweight Bout</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
+          <t>9:39</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>49%</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Jul 24, 1995</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>6' 2"</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>http://ufcstats.com/fighter-details/a93f94c923c3a9cb</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>"CLD"</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>79"</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>3.57</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>4.71</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>62%</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>14%</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>64%</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>185 lbs.</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>10-2-0</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
           <t>15:00</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>47%</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>Sep 10, 1997</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>6' 4"</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>http://ufcstats.com/fighter-details/22e07d3da1aa3475</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>78"</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>Southpaw</t>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>6.53</t>
+        </is>
+      </c>
+      <c r="AJ11" t="inlineStr">
         <is>
           <t>68%</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Dec 16, 1999</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>5' 6"</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>http://ufcstats.com/fighter-details/1b35af4d1529adf6</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>"Rondinha"</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>65"</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>Orthodox</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>2.53</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>5.30</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>48%</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
+      <c r="AK11" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>85%</t>
-        </is>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>0.50</t>
-        </is>
-      </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>115 lbs.</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>6-1-1</t>
-        </is>
-      </c>
-      <c r="Z11" t="inlineStr">
-        <is>
-          <t>13:46</t>
-        </is>
-      </c>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>56%</t>
-        </is>
-      </c>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>Jun 28, 1992</t>
-        </is>
-      </c>
-      <c r="AC11" t="inlineStr">
-        <is>
-          <t>5' 5"</t>
-        </is>
-      </c>
-      <c r="AD11" t="inlineStr">
-        <is>
-          <t>http://ufcstats.com/fighter-details/e94085e821bd81de</t>
-        </is>
-      </c>
-      <c r="AE11" t="inlineStr">
-        <is>
-          <t>"Sampage"</t>
-        </is>
-      </c>
-      <c r="AF11" t="inlineStr">
-        <is>
-          <t>64"</t>
-        </is>
-      </c>
-      <c r="AG11" t="inlineStr">
-        <is>
-          <t>Orthodox</t>
-        </is>
-      </c>
-      <c r="AH11" t="inlineStr">
-        <is>
-          <t>4.46</t>
-        </is>
-      </c>
-      <c r="AI11" t="inlineStr">
-        <is>
-          <t>4.33</t>
-        </is>
-      </c>
-      <c r="AJ11" t="inlineStr">
-        <is>
-          <t>46%</t>
-        </is>
-      </c>
-      <c r="AK11" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="AM11" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="AN11" t="inlineStr">
         <is>
-          <t>0.85</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="AO11" t="inlineStr">
         <is>
-          <t>115 lbs.</t>
+          <t>185 lbs.</t>
         </is>
       </c>
       <c r="AP11" t="inlineStr">
         <is>
-          <t>9-6-0</t>
+          <t>9-2-0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/5d8af316413ea2f7</t>
+          <t>http://ufcstats.com/fight-details/a693622ad8c0d672</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Daniel Barez</t>
+          <t>Shauna Bannon</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Andre Lima</t>
+          <t>Puja Tomar</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Flyweight Bout</t>
+          <t>Women's Strawweight Bout</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>11:09</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>57%</t>
+          <t>42%</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Dec 10, 1988</t>
+          <t>Oct 23, 1993</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>5' 6"</t>
+          <t>5' 5"</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/e8fe9c15d348e778</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr"/>
+          <t>http://ufcstats.com/fighter-details/9c442aaf149ea982</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>"Mama B"</t>
+        </is>
+      </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>66"</t>
+          <t>65"</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Orthodox</t>
+          <t>Switch</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>5.05</t>
+          <t>3.77</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>4.10</t>
+          <t>4.37</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>52%</t>
+          <t>41%</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>31%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>42%</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>2.24</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>125 lbs.</t>
+          <t>115 lbs.</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>17-6-0</t>
+          <t>6-1-0</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>57%</t>
+          <t>44%</t>
         </is>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>Feb 04, 1999</t>
+          <t>Dec 05, 1993</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
         <is>
-          <t>5' 7"</t>
+          <t>5' 4"</t>
         </is>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/b1f21ce050035d58</t>
+          <t>http://ufcstats.com/fighter-details/19f8a2f6eecd92ac</t>
         </is>
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>"Mascote"</t>
+          <t>"Cyclone"</t>
         </is>
       </c>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>67"</t>
+          <t>59"</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr">
         <is>
-          <t>Orthodox</t>
+          <t>Southpaw</t>
         </is>
       </c>
       <c r="AH12" t="inlineStr">
         <is>
-          <t>2.48</t>
+          <t>5.60</t>
         </is>
       </c>
       <c r="AI12" t="inlineStr">
         <is>
-          <t>3.03</t>
+          <t>6.33</t>
         </is>
       </c>
       <c r="AJ12" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>47%</t>
         </is>
       </c>
       <c r="AK12" t="inlineStr">
         <is>
-          <t>1.1</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AL12" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="AM12" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="AN12" t="inlineStr">
         <is>
-          <t>1.13</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AO12" t="inlineStr">
         <is>
-          <t>125 lbs.</t>
+          <t>115 lbs.</t>
         </is>
       </c>
       <c r="AP12" t="inlineStr">
         <is>
-          <t>10-0-0</t>
+          <t>9-4-0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/1c62a7444808d97f</t>
+          <t>http://ufcstats.com/fight-details/1b02588149d126bf</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Josiane Nunes</t>
+          <t>Nathan Fletcher</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Priscila Cachoeira</t>
+          <t>Caolan Loughran</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Women's Bantamweight Bout</t>
+          <t>Bantamweight Bout</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>12:59</t>
+          <t>6:14</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>51%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Dec 23, 1993</t>
+          <t>Jan 03, 1998</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>5' 2"</t>
+          <t>5' 7"</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/68d35296f566792b</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>"Josi"</t>
-        </is>
-      </c>
+          <t>http://ufcstats.com/fighter-details/a2d342ffc83913ed</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
-          <t>67"</t>
+          <t>70"</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Southpaw</t>
+          <t>Orthodox</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>5.44</t>
+          <t>0.96</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>5.41</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>42%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
+          <t>2.4</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>66%</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>9.63</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>135 lbs.</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>9-1-0</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>54%</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>May 18, 1996</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>5' 6"</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>http://ufcstats.com/fighter-details/42ac4020cba261ad</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>"The Don"</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>68"</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>Orthodox</t>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>5.62</t>
+        </is>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t>5.64</t>
+        </is>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>43%</t>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>58%</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X13" t="inlineStr">
+      <c r="AL13" t="inlineStr">
+        <is>
+          <t>26%</t>
+        </is>
+      </c>
+      <c r="AM13" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="AN13" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="AO13" t="inlineStr">
         <is>
           <t>135 lbs.</t>
         </is>
       </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>10-3-0</t>
-        </is>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>9:45</t>
-        </is>
-      </c>
-      <c r="AA13" t="inlineStr">
-        <is>
-          <t>43%</t>
-        </is>
-      </c>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>Aug 19, 1988</t>
-        </is>
-      </c>
-      <c r="AC13" t="inlineStr">
-        <is>
-          <t>5' 7"</t>
-        </is>
-      </c>
-      <c r="AD13" t="inlineStr">
-        <is>
-          <t>http://ufcstats.com/fighter-details/b1e5bcaad32a3cac</t>
-        </is>
-      </c>
-      <c r="AE13" t="inlineStr">
-        <is>
-          <t>"Zombie Girl"</t>
-        </is>
-      </c>
-      <c r="AF13" t="inlineStr">
-        <is>
-          <t>65"</t>
-        </is>
-      </c>
-      <c r="AG13" t="inlineStr">
-        <is>
-          <t>Orthodox</t>
-        </is>
-      </c>
-      <c r="AH13" t="inlineStr">
-        <is>
-          <t>7.03</t>
-        </is>
-      </c>
-      <c r="AI13" t="inlineStr">
-        <is>
-          <t>3.76</t>
-        </is>
-      </c>
-      <c r="AJ13" t="inlineStr">
-        <is>
-          <t>44%</t>
-        </is>
-      </c>
-      <c r="AK13" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="AL13" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
-      </c>
-      <c r="AM13" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
-      </c>
-      <c r="AN13" t="inlineStr">
-        <is>
-          <t>0.15</t>
-        </is>
-      </c>
-      <c r="AO13" t="inlineStr">
-        <is>
-          <t>135 lbs.</t>
-        </is>
-      </c>
       <c r="AP13" t="inlineStr">
         <is>
-          <t>12-6-0</t>
+          <t>9-2-0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UFC Fight Night: Vettori vs. Dolidze 2</t>
+          <t>UFC Fight Night: Edwards vs. Brady</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>March 15, 2025</t>
+          <t>March 22, 2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Las Vegas, Nevada, USA</t>
+          <t>London, England, United Kingdom</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/event-details/39f62b833e4cf126</t>
+          <t>http://ufcstats.com/event-details/cc2ad11b1f9d818b</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fight-details/a8f8245096eaf0cd</t>
+          <t>http://ufcstats.com/fight-details/265dbd9be8caa7de</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Yuneisy Duben</t>
+          <t>Guram Kutateladze</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Carli Judice</t>
+          <t>Kaue Fernandes</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Women's Flyweight Bout</t>
+          <t>Lightweight Bout</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1:13</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>41%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Jul 08, 1996</t>
+          <t>Jan 08, 1992</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>5' 4"</t>
+          <t>5' 11"</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/c3d2b9bcb4cead6b</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr"/>
+          <t>http://ufcstats.com/fighter-details/7772b283d288dbe2</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>"Georgian Viking"</t>
+        </is>
+      </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>65"</t>
+          <t>72"</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -3256,17 +3248,17 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>11.51</t>
+          <t>3.95</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>20.55</t>
+          <t>3.95</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>64%</t>
+          <t>45%</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
@@ -3276,82 +3268,78 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>20%</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.77</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>125 lbs.</t>
+          <t>155 lbs.</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>6-0-0 (1 NC)</t>
+          <t>13-4-0</t>
         </is>
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>9:53</t>
         </is>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>52%</t>
+          <t>66%</t>
         </is>
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>Mar 02, 1999</t>
+          <t>Mar 17, 1995</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>5' 7"</t>
+          <t>5' 9"</t>
         </is>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>http://ufcstats.com/fighter-details/f1ab6f37492c630a</t>
-        </is>
-      </c>
-      <c r="AE14" t="inlineStr">
-        <is>
-          <t>"Crispy"</t>
-        </is>
-      </c>
+          <t>http://ufcstats.com/fighter-details/ec13c393d029297d</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>68"</t>
+          <t>73"</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr">
         <is>
-          <t>Southpaw</t>
+          <t>Orthodox</t>
         </is>
       </c>
       <c r="AH14" t="inlineStr">
         <is>
-          <t>10.10</t>
+          <t>0.86</t>
         </is>
       </c>
       <c r="AI14" t="inlineStr">
         <is>
-          <t>11.23</t>
+          <t>3.04</t>
         </is>
       </c>
       <c r="AJ14" t="inlineStr">
         <is>
-          <t>54%</t>
+          <t>57%</t>
         </is>
       </c>
       <c r="AK14" t="inlineStr">
@@ -3361,27 +3349,27 @@
       </c>
       <c r="AL14" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="AM14" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="AN14" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>0.76</t>
         </is>
       </c>
       <c r="AO14" t="inlineStr">
         <is>
-          <t>125 lbs.</t>
+          <t>155 lbs.</t>
         </is>
       </c>
       <c r="AP14" t="inlineStr">
         <is>
-          <t>3-2-0</t>
+          <t>9-2-0</t>
         </is>
       </c>
     </row>

</xml_diff>